<commit_message>
Latest version - Added feedback controls + database connection
</commit_message>
<xml_diff>
--- a/Welcome_Screen/Database code/fakeRFIDdata.xlsx
+++ b/Welcome_Screen/Database code/fakeRFIDdata.xlsx
@@ -21,6 +21,59 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>Deutsche Bank</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Guntram</t>
+  </si>
+  <si>
+    <t>Schmitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heinrich </t>
+  </si>
+  <si>
+    <t>Vogel</t>
+  </si>
+  <si>
+    <t>Sparkasse</t>
+  </si>
+  <si>
+    <t>Commerzbank</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,12 +423,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>